<commit_message>
Refactor email code into class
</commit_message>
<xml_diff>
--- a/rates/output.xlsx
+++ b/rates/output.xlsx
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -450,12 +450,12 @@
       <c r="F1" t="inlineStr"/>
       <c r="G1" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.2035</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>862.73</t>
+          <t>858.0955</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -467,7 +467,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -493,12 +493,12 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.2035</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>4451.59</t>
+          <t>4427.6765000000005</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -510,7 +510,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -536,12 +536,12 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.2035</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>29.060086</t>
+          <t>28.9039781</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -553,7 +553,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -579,12 +579,12 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.2035</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>23.716</t>
+          <t>23.588600000000003</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -596,7 +596,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -622,12 +622,12 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.2035</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>8107.0</t>
+          <t>8063.45</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -639,7 +639,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -665,12 +665,12 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.2035</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4.4649</t>
+          <t>4.440915</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -682,7 +682,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -708,12 +708,12 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.2035</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>68.58279999999999</t>
+          <t>68.21438</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -725,7 +725,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -751,12 +751,12 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.2035</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>68.2198</t>
+          <t>67.85333</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -768,7 +768,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -790,7 +790,7 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.2035</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -803,7 +803,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -830,7 +830,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -853,7 +853,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>

</xml_diff>